<commit_message>
Updated Readme.md for Python projects and etc.
Added requirements.txt
Updated comments in excel_rtd_server.py
Set FINNHUB RTD's default value to "N/A"
</commit_message>
<xml_diff>
--- a/python/demo/Finnhub_rtd_demo.xlsx
+++ b/python/demo/Finnhub_rtd_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\GitHub\ExcelRTD\python\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EF2B47-5AB0-406A-AE7B-FD94B750F614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868B00BE-0239-4119-AD1F-EA27FBFE0D68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="1545" windowWidth="15480" windowHeight="12675" xr2:uid="{E4C61899-80CC-4189-A1D7-D7852CB17CA7}"/>
+    <workbookView xWindow="7245" yWindow="2475" windowWidth="21600" windowHeight="11250" xr2:uid="{E4C61899-80CC-4189-A1D7-D7852CB17CA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Finnhub RTD Demo" sheetId="1" r:id="rId1"/>
@@ -153,148 +153,182 @@
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
     <main first="finnhub">
-      <tp t="e">
-        <v>#N/A</v>
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>BINANCE:ETHBTC</stp>
         <stp>last_update_time</stp>
         <tr r="D5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>FB</stp>
         <stp>volume</stp>
         <tr r="C10" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>BINANCE:BTCUSDT</stp>
         <stp>last_update_time</stp>
         <tr r="D4" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>MSFT</stp>
         <stp>volume</stp>
         <tr r="C6" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>MSFT</stp>
         <stp>last_update_time</stp>
         <tr r="D6" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>GOOG</stp>
         <stp>volume</stp>
         <tr r="C9" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>AAPL</stp>
         <stp>volume</stp>
         <tr r="C7" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>AMZN</stp>
         <stp>volume</stp>
         <tr r="C8" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>GOOG</stp>
         <stp>last_update_time</stp>
         <tr r="D9" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>AAPL</stp>
         <stp>last_update_time</stp>
         <tr r="D7" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>BINANCE:BTCUSDT</stp>
         <stp>last_price</stp>
         <tr r="B4" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>AMZN</stp>
         <stp>last_update_time</stp>
         <tr r="D8" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>BINANCE:ETHBTC</stp>
         <stp>last_price</stp>
         <tr r="B5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>MSFT</stp>
         <stp>last_price</stp>
         <tr r="B6" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>AMZN</stp>
         <stp>last_price</stp>
         <tr r="B8" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>AAPL</stp>
         <stp>last_price</stp>
         <tr r="B7" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>GOOG</stp>
         <stp>last_price</stp>
         <tr r="B9" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>FB</stp>
         <stp>last_update_time</stp>
         <tr r="D10" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>BINANCE:ETHBTC</stp>
         <stp>volume</stp>
         <tr r="C5" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>BINANCE:BTCUSDT</stp>
         <stp>volume</stp>
         <tr r="C4" s="1"/>
       </tp>
-      <tp t="e">
-        <v>#N/A</v>
+    </main>
+    <main first="finnhub">
+      <tp>
+        <v>0</v>
         <stp/>
         <stp>FB</stp>
         <stp>last_price</stp>
@@ -624,7 +658,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,8 +672,8 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="str">
-        <f>IF(A1="","Copy paste your Finnhub token to A1 cell",RTD("finnhub","","set_token",A1))</f>
-        <v>Copy paste your Finnhub token to A1 cell</v>
+        <f>IF(A1="","&lt;--Copy paste your Finnhub API key to A1 cell. Go to https://finnhub.io/dashboard to get your API key.",RTD("finnhub","","set_token",A1))</f>
+        <v>&lt;--Copy paste your Finnhub API key to A1 cell. Go to https://finnhub.io/dashboard to get your API key.</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -662,15 +696,15 @@
       </c>
       <c r="B4" s="1">
         <f>RTD("finnhub","",A4,"last_price")</f>
-        <v>9163.85</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>RTD("finnhub","",A4,"volume")</f>
-        <v>1.0683E-2</v>
-      </c>
-      <c r="D4" t="str">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <f>RTD("finnhub","",A4,"last_update_time")</f>
-        <v>2020-07-17 17:16:27.285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -679,15 +713,15 @@
       </c>
       <c r="B5" s="2">
         <f>RTD("finnhub","",A5,"last_price")</f>
-        <v>2.5440000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3">
         <f>RTD("finnhub","",A5,"volume")</f>
-        <v>1.2749999999999999</v>
-      </c>
-      <c r="D5" t="str">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <f>RTD("finnhub","",A5,"last_update_time")</f>
-        <v>2020-07-17 17:16:28.999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,15 +730,15 @@
       </c>
       <c r="B6" s="1">
         <f>RTD("finnhub","",A6,"last_price")</f>
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>RTD("finnhub","",A6,"volume")</f>
-        <v>50</v>
-      </c>
-      <c r="D6" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6">
         <f>RTD("finnhub","",A6,"last_update_time")</f>
-        <v>2020-07-17 16:55:33.935</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -713,15 +747,15 @@
       </c>
       <c r="B7" s="1">
         <f>RTD("finnhub","",A7,"last_price")</f>
-        <v>385.45</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f>RTD("finnhub","",A7,"volume")</f>
-        <v>10</v>
-      </c>
-      <c r="D7" t="str">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <f>RTD("finnhub","",A7,"last_update_time")</f>
-        <v>2020-07-17 16:55:36.587</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>